<commit_message>
Passed adjacency and target tests
</commit_message>
<xml_diff>
--- a/ClueBoard.xlsx
+++ b/ClueBoard.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1000,9 +1000,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1670,7 +1668,7 @@
       <c r="H9" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="I9" s="48" t="s">
+      <c r="I9" s="5" t="s">
         <v>25</v>
       </c>
       <c r="J9" s="5" t="s">
@@ -1745,7 +1743,7 @@
       <c r="H10" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="I10" s="5" t="s">
+      <c r="I10" s="48" t="s">
         <v>25</v>
       </c>
       <c r="J10" s="5" t="s">

</xml_diff>

<commit_message>
Refactored disproveSuggestion to player, not computerPlayer, created failing tests for handling suggestions
</commit_message>
<xml_diff>
--- a/ClueBoard.xlsx
+++ b/ClueBoard.xlsx
@@ -1000,7 +1000,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>